<commit_message>
Add benchamrk results cp3
</commit_message>
<xml_diff>
--- a/reports/data_report_2.xlsx
+++ b/reports/data_report_2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="165">
   <si>
     <t>OMP_NUM_THREADS=1</t>
   </si>
@@ -358,6 +358,168 @@
   </si>
   <si>
     <t>10.246</t>
+  </si>
+  <si>
+    <t>0.028</t>
+  </si>
+  <si>
+    <t>0.185</t>
+  </si>
+  <si>
+    <t>0.424</t>
+  </si>
+  <si>
+    <t>1.014</t>
+  </si>
+  <si>
+    <t>0.048</t>
+  </si>
+  <si>
+    <t>0.051</t>
+  </si>
+  <si>
+    <t>0.113</t>
+  </si>
+  <si>
+    <t>0.853</t>
+  </si>
+  <si>
+    <t>1.835</t>
+  </si>
+  <si>
+    <t>4.223</t>
+  </si>
+  <si>
+    <t>0.208</t>
+  </si>
+  <si>
+    <t>0.217</t>
+  </si>
+  <si>
+    <t>0.447</t>
+  </si>
+  <si>
+    <t>3.758</t>
+  </si>
+  <si>
+    <t>7.659</t>
+  </si>
+  <si>
+    <t>17.163</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.096</t>
+  </si>
+  <si>
+    <t>0.234</t>
+  </si>
+  <si>
+    <t>0.566</t>
+  </si>
+  <si>
+    <t>0.026</t>
+  </si>
+  <si>
+    <t>0.057</t>
+  </si>
+  <si>
+    <t>0.480</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>2.272</t>
+  </si>
+  <si>
+    <t>0.108</t>
+  </si>
+  <si>
+    <t>0.225</t>
+  </si>
+  <si>
+    <t>2.068</t>
+  </si>
+  <si>
+    <t>4.041</t>
+  </si>
+  <si>
+    <t>9.066</t>
+  </si>
+  <si>
+    <t>0.073</t>
+  </si>
+  <si>
+    <t>0.432</t>
+  </si>
+  <si>
+    <t>0.042</t>
+  </si>
+  <si>
+    <t>0.294</t>
+  </si>
+  <si>
+    <t>0.570</t>
+  </si>
+  <si>
+    <t>1.229</t>
+  </si>
+  <si>
+    <t>0.064</t>
+  </si>
+  <si>
+    <t>0.076</t>
+  </si>
+  <si>
+    <t>0.120</t>
+  </si>
+  <si>
+    <t>1.116</t>
+  </si>
+  <si>
+    <t>2.259</t>
+  </si>
+  <si>
+    <t>4.926</t>
+  </si>
+  <si>
+    <t>0.043</t>
+  </si>
+  <si>
+    <t>0.106</t>
+  </si>
+  <si>
+    <t>0.216</t>
+  </si>
+  <si>
+    <t>0.024</t>
+  </si>
+  <si>
+    <t>0.184</t>
+  </si>
+  <si>
+    <t>0.427</t>
+  </si>
+  <si>
+    <t>0.859</t>
+  </si>
+  <si>
+    <t>0.092</t>
+  </si>
+  <si>
+    <t>0.742</t>
+  </si>
+  <si>
+    <t>1.713</t>
+  </si>
+  <si>
+    <t>3.513</t>
+  </si>
+  <si>
+    <t>Vectorised Code</t>
   </si>
 </sst>
 </file>
@@ -428,7 +590,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -504,8 +666,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -515,8 +687,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -554,6 +729,11 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -591,6 +771,11 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -868,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
@@ -1473,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,9 +2533,861 @@
         <v>110</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>100</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1000</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>2000</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F57" t="s">
+        <v>58</v>
+      </c>
+      <c r="G57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>4000</v>
+      </c>
+      <c r="D58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" t="s">
+        <v>58</v>
+      </c>
+      <c r="G59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>58</v>
+      </c>
+      <c r="F60" t="s">
+        <v>58</v>
+      </c>
+      <c r="G60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>100</v>
+      </c>
+      <c r="D61" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" t="s">
+        <v>58</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>1000</v>
+      </c>
+      <c r="D62" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>2000</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>58</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64">
+        <v>10</v>
+      </c>
+      <c r="C64">
+        <v>4000</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>58</v>
+      </c>
+      <c r="G64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" t="s">
+        <v>58</v>
+      </c>
+      <c r="F65" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66">
+        <v>100</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
+        <v>58</v>
+      </c>
+      <c r="F66" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67">
+        <v>100</v>
+      </c>
+      <c r="C67">
+        <v>100</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>58</v>
+      </c>
+      <c r="G67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68">
+        <v>100</v>
+      </c>
+      <c r="C68">
+        <v>1000</v>
+      </c>
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>2</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69">
+        <v>100</v>
+      </c>
+      <c r="C69">
+        <v>2000</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2</v>
+      </c>
+      <c r="G69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70">
+        <v>100</v>
+      </c>
+      <c r="C70">
+        <v>4000</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71">
+        <v>1000</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B72">
+        <v>1000</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73">
+        <v>1000</v>
+      </c>
+      <c r="C73">
+        <v>100</v>
+      </c>
+      <c r="D73" t="s">
+        <v>111</v>
+      </c>
+      <c r="E73" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74">
+        <v>1000</v>
+      </c>
+      <c r="C74">
+        <v>1000</v>
+      </c>
+      <c r="D74" t="s">
+        <v>112</v>
+      </c>
+      <c r="E74" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" t="s">
+        <v>141</v>
+      </c>
+      <c r="G74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75">
+        <v>1000</v>
+      </c>
+      <c r="C75">
+        <v>2000</v>
+      </c>
+      <c r="D75" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" t="s">
+        <v>129</v>
+      </c>
+      <c r="F75" t="s">
+        <v>50</v>
+      </c>
+      <c r="G75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76">
+        <v>1000</v>
+      </c>
+      <c r="C76">
+        <v>4000</v>
+      </c>
+      <c r="D76" t="s">
+        <v>114</v>
+      </c>
+      <c r="E76" t="s">
+        <v>130</v>
+      </c>
+      <c r="F76" t="s">
+        <v>142</v>
+      </c>
+      <c r="G76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>57</v>
+      </c>
+      <c r="B77">
+        <v>2000</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>115</v>
+      </c>
+      <c r="E77" t="s">
+        <v>131</v>
+      </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78">
+        <v>2000</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78" t="s">
+        <v>116</v>
+      </c>
+      <c r="E78" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>2000</v>
+      </c>
+      <c r="C79">
+        <v>100</v>
+      </c>
+      <c r="D79" t="s">
+        <v>117</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+      <c r="F79" t="s">
+        <v>143</v>
+      </c>
+      <c r="G79" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80">
+        <v>2000</v>
+      </c>
+      <c r="C80">
+        <v>1000</v>
+      </c>
+      <c r="D80" t="s">
+        <v>118</v>
+      </c>
+      <c r="E80" t="s">
+        <v>133</v>
+      </c>
+      <c r="F80" t="s">
+        <v>144</v>
+      </c>
+      <c r="G80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81">
+        <v>2000</v>
+      </c>
+      <c r="C81">
+        <v>2000</v>
+      </c>
+      <c r="D81" t="s">
+        <v>119</v>
+      </c>
+      <c r="E81" t="s">
+        <v>134</v>
+      </c>
+      <c r="F81" t="s">
+        <v>145</v>
+      </c>
+      <c r="G81" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>57</v>
+      </c>
+      <c r="B82">
+        <v>2000</v>
+      </c>
+      <c r="C82">
+        <v>4000</v>
+      </c>
+      <c r="D82" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" t="s">
+        <v>135</v>
+      </c>
+      <c r="F82" t="s">
+        <v>146</v>
+      </c>
+      <c r="G82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83">
+        <v>4000</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>121</v>
+      </c>
+      <c r="E83" t="s">
+        <v>136</v>
+      </c>
+      <c r="F83" t="s">
+        <v>147</v>
+      </c>
+      <c r="G83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84">
+        <v>4000</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>122</v>
+      </c>
+      <c r="E84" t="s">
+        <v>85</v>
+      </c>
+      <c r="F84" t="s">
+        <v>148</v>
+      </c>
+      <c r="G84" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85">
+        <v>4000</v>
+      </c>
+      <c r="C85">
+        <v>100</v>
+      </c>
+      <c r="D85" t="s">
+        <v>123</v>
+      </c>
+      <c r="E85" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85" t="s">
+        <v>149</v>
+      </c>
+      <c r="G85" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86">
+        <v>4000</v>
+      </c>
+      <c r="C86">
+        <v>1000</v>
+      </c>
+      <c r="D86" t="s">
+        <v>124</v>
+      </c>
+      <c r="E86" t="s">
+        <v>138</v>
+      </c>
+      <c r="F86" t="s">
+        <v>150</v>
+      </c>
+      <c r="G86" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87">
+        <v>4000</v>
+      </c>
+      <c r="C87">
+        <v>2000</v>
+      </c>
+      <c r="D87" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87" t="s">
+        <v>139</v>
+      </c>
+      <c r="F87" t="s">
+        <v>151</v>
+      </c>
+      <c r="G87" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88">
+        <v>4000</v>
+      </c>
+      <c r="C88">
+        <v>4000</v>
+      </c>
+      <c r="D88" t="s">
+        <v>126</v>
+      </c>
+      <c r="E88" t="s">
+        <v>140</v>
+      </c>
+      <c r="F88" t="s">
+        <v>152</v>
+      </c>
+      <c r="G88" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C47:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>